<commit_message>
update spec fonctionelles, pdf et solution technique
</commit_message>
<xml_diff>
--- a/pdf/src/UseCaseDetails.xlsx
+++ b/pdf/src/UseCaseDetails.xlsx
@@ -480,10 +480,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,10 +800,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -864,10 +864,10 @@
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
@@ -1010,8 +1010,8 @@
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
@@ -1034,10 +1034,10 @@
       <c r="C33" s="4"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="8"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
@@ -1092,10 +1092,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1156,10 +1156,10 @@
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
@@ -1265,7 +1265,7 @@
       <c r="B25" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1273,13 +1273,13 @@
       <c r="B26" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -1304,10 +1304,10 @@
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="8"/>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" spans="2:3" ht="192.75" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
@@ -1349,7 +1349,7 @@
   <dimension ref="B2:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="B2:C32"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,10 +1361,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1425,10 +1425,10 @@
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
@@ -1510,7 +1510,7 @@
       <c r="B22" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1526,13 +1526,13 @@
       <c r="B24" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
@@ -1557,10 +1557,10 @@
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="8"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" spans="2:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -1594,5 +1594,6 @@
     <mergeCell ref="B25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update with correction according to the evaluator s feedback
</commit_message>
<xml_diff>
--- a/pdf/src/UseCaseDetails.xlsx
+++ b/pdf/src/UseCaseDetails.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="135" windowWidth="20115" windowHeight="9525" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="135" windowWidth="20115" windowHeight="9525" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="141">
   <si>
     <t>Cas n° 1</t>
   </si>
@@ -407,6 +408,80 @@
   <si>
     <t>L'activation/désactivation manuelle d'un produit est prioritaire sur le traitement automatique. 
 Souhaitez-vous un reporting quotidien indiquant les mouvements de visibilité produit afin de pouvoir détecter (et rectifier le cas échéant) les erreurs de stock ou les oublis d'activation/de désactivation produit ?</t>
+  </si>
+  <si>
+    <t>Cas n° 4</t>
+  </si>
+  <si>
+    <t>S'identifie sur le site - Client (Package "PDV")</t>
+  </si>
+  <si>
+    <t>Identification de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Rémy VALLET (22/12/2019)</t>
+  </si>
+  <si>
+    <t>○ L'utilisateur à créé un compte sur le site
+○ L'utilisateur possède un point de vente préféré</t>
+  </si>
+  <si>
+    <t>Le client arrive sur la page d'identification</t>
+  </si>
+  <si>
+    <t>L'utilisateur saisie son identifiant (eMail) et son mot de passe</t>
+  </si>
+  <si>
+    <t>Le système interroge via une connexion sécurisé la correspondance en base de données.</t>
+  </si>
+  <si>
+    <t>Le système renvoie une autorisation temporaire pour une session à durée limitée (expiration token)</t>
+  </si>
+  <si>
+    <t>L'utilisateur est redirigé en page d'accueil, le catalogue produit du point de vente du profile chargé, une animation au niveau de l'icone d'identification lui confirme sa connexion (layer "connexion réussie")</t>
+  </si>
+  <si>
+    <t>L'utilisateur ne connais pas son mot de passe</t>
+  </si>
+  <si>
+    <t>L'utilisateur est invité à cliquer sur un lien "mot de passe oublié"</t>
+  </si>
+  <si>
+    <t>1c.</t>
+  </si>
+  <si>
+    <t>Le système affiche une page permettant de saisir un email et un bouton récupérer l'accès à mon compte</t>
+  </si>
+  <si>
+    <t>1d.</t>
+  </si>
+  <si>
+    <t>Si le système trouve une correspondance utilisateur, il renvoie un email avec un lien contenant un jeton temporaire d'accès à la modification de mot de passe.</t>
+  </si>
+  <si>
+    <t>1e.</t>
+  </si>
+  <si>
+    <t>Si le système ne trouve pas de correspondance, l'utilisateur est invité à créer un compte.</t>
+  </si>
+  <si>
+    <t>○ Scénario nominal point 4</t>
+  </si>
+  <si>
+    <t>L'utilisateur effectue une double saisie de son nouveau de passe et accède à son compte.</t>
+  </si>
+  <si>
+    <t>○ L'utilisateur visualise à chaque action la réussite ou l'échec de l'action (layer/popin en affichage temporaire).</t>
+  </si>
+  <si>
+    <t>○ Envoie rapide du lien de réinitialisation du mot de passe
+○ Un affichage intuitif de la réussite ou de l'echec d'une action</t>
+  </si>
+  <si>
+    <t>Comment gérer les tentatives de saturation de demande de réinitialisation de mot de passe ? Seriez-vous d'accord pour bannir sur une durée limité les ips effectuants des demande de réinitialisation de mot de passe (ex : 5 tentatives succéssives -&gt; IP bannie pendant 24H ?)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1348,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,4 +1671,247 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.5703125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="24" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B24:C24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>